<commit_message>
Update sample fastq file paths to dev bucket gcloud location instead of SRA
</commit_message>
<xml_diff>
--- a/config/config-sra-test-subset.xlsx
+++ b/config/config-sra-test-subset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cherikhsr/Documents/GitHub/cidc_atac/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680E42F3-1293-F54F-9CD1-0B5FD232443A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA79208-4DDA-0B42-8A38-BF70546852EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="30180" windowHeight="26500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="30180" windowHeight="26500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="180">
   <si>
     <t>&lt;string&gt;</t>
   </si>
@@ -1559,12 +1559,6 @@
     <t>wt</t>
   </si>
   <si>
-    <t>SRR16579104</t>
-  </si>
-  <si>
-    <t>SRR16579106</t>
-  </si>
-  <si>
     <t>A549</t>
   </si>
   <si>
@@ -1612,13 +1606,25 @@
   </si>
   <si>
     <t>benchmark log info progress genome annot input cutadapt rqual_filter bam rseqc fastqc cnv peak chipqc</t>
+  </si>
+  <si>
+    <t>gs://chips2-test-data/atac-test-sample-fastq/SRR16579104_1.fastq.gz</t>
+  </si>
+  <si>
+    <t>gs://chips2-test-data/atac-test-sample-fastq/SRR16579106_1.fastq.gz</t>
+  </si>
+  <si>
+    <t>gs://chips2-test-data/atac-test-sample-fastq/SRR16579104_2.fastq.gz</t>
+  </si>
+  <si>
+    <t>gs://chips2-test-data/atac-test-sample-fastq/SRR16579106_2.fastq.gz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1666,6 +1672,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1744,7 +1757,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1814,6 +1827,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2120,8 +2134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7:P9"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2139,7 +2153,7 @@
     <col min="13" max="13" width="86.6640625" customWidth="1"/>
     <col min="14" max="14" width="85.1640625" customWidth="1"/>
     <col min="15" max="15" width="67.33203125" customWidth="1"/>
-    <col min="16" max="16" width="47.1640625" customWidth="1"/>
+    <col min="16" max="16" width="55.5" customWidth="1"/>
     <col min="17" max="17" width="44.1640625" customWidth="1"/>
     <col min="18" max="18" width="42" customWidth="1"/>
   </cols>
@@ -2173,7 +2187,7 @@
         <v>60</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>158</v>
@@ -2230,10 +2244,10 @@
         <v>37</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>39</v>
@@ -2245,7 +2259,7 @@
         <v>41</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="P2" s="7" t="s">
         <v>20</v>
@@ -2322,7 +2336,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -2335,11 +2349,11 @@
       <c r="M4" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="O4" t="s">
-        <v>164</v>
-      </c>
-      <c r="P4" t="s">
-        <v>164</v>
+      <c r="O4" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="P4" s="27" t="s">
+        <v>178</v>
       </c>
       <c r="Q4" s="26"/>
     </row>
@@ -2350,7 +2364,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -2363,11 +2377,11 @@
       <c r="M5" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="O5" t="s">
-        <v>165</v>
-      </c>
-      <c r="P5" t="s">
-        <v>165</v>
+      <c r="O5" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="P5" s="27" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
@@ -2379,6 +2393,7 @@
       <c r="I6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="2"/>
+      <c r="O6" s="27"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
@@ -2389,6 +2404,7 @@
       <c r="I7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="2"/>
+      <c r="O7" s="27"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
@@ -2399,6 +2415,7 @@
       <c r="I8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="2"/>
+      <c r="O8" s="27"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
@@ -2409,6 +2426,7 @@
       <c r="I9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="2"/>
+      <c r="O9" s="27"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
@@ -2631,7 +2649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -2661,7 +2679,7 @@
         <v>80</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -2672,7 +2690,7 @@
         <v>116</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2725,7 +2743,7 @@
         <v>150</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -2741,10 +2759,10 @@
     </row>
     <row r="10" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C10" s="6">
         <v>37</v>
@@ -2791,7 +2809,7 @@
         <v>139</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2980,7 +2998,7 @@
         <v>81</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update some peak calling params that are called with macs
Using params (shift, ext_size) which seem to be commonly used for calling peaks with ATACseq data.
</commit_message>
<xml_diff>
--- a/config/config-sra-test-subset.xlsx
+++ b/config/config-sra-test-subset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cherikhsr/Documents/GitHub/cidc_atac/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA79208-4DDA-0B42-8A38-BF70546852EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC216416-8A72-BC48-AF23-C6DD3CC20CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="30180" windowHeight="26500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="30180" windowHeight="26500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -2134,7 +2134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
@@ -2649,8 +2649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2754,7 +2754,7 @@
         <v>152</v>
       </c>
       <c r="C9" s="6">
-        <v>73</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="64" x14ac:dyDescent="0.2">
@@ -2765,7 +2765,7 @@
         <v>171</v>
       </c>
       <c r="C10" s="6">
-        <v>37</v>
+        <v>-75</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -2776,7 +2776,7 @@
         <v>155</v>
       </c>
       <c r="C11" s="6">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="48" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add arg in config to run genomic tracks or not
May need to add other args for regions / genes for the tracks
</commit_message>
<xml_diff>
--- a/config/config-sra-test-subset.xlsx
+++ b/config/config-sra-test-subset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cherikhsr/Documents/GitHub/cidc_atac/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC216416-8A72-BC48-AF23-C6DD3CC20CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59F5217-B2FD-EA4F-8508-EAE8B5A952A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="500" windowWidth="30180" windowHeight="26500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1046,25 +1046,6 @@
     <t>cloud_prog</t>
   </si>
   <si>
-    <t>save_unmapped</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Flag to save un aligned reads in a fastq file. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Available options: 0;1   (REQUIRED)</t>
-    </r>
-  </si>
-  <si>
     <t>bwa_prog</t>
   </si>
   <si>
@@ -1562,9 +1543,6 @@
     <t>A549</t>
   </si>
   <si>
-    <t>broad</t>
-  </si>
-  <si>
     <t>Sample Replicate</t>
   </si>
   <si>
@@ -1618,6 +1596,28 @@
   </si>
   <si>
     <t>gs://chips2-test-data/atac-test-sample-fastq/SRR16579106_2.fastq.gz</t>
+  </si>
+  <si>
+    <t>run_genome_track</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Generate genomic track files and images. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Available options: 0;1   (REQUIRED)</t>
+    </r>
+  </si>
+  <si>
+    <t>narrow</t>
   </si>
 </sst>
 </file>
@@ -2187,10 +2187,10 @@
         <v>60</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>61</v>
@@ -2244,10 +2244,10 @@
         <v>37</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>39</v>
@@ -2259,7 +2259,7 @@
         <v>41</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="P2" s="7" t="s">
         <v>20</v>
@@ -2331,12 +2331,12 @@
     </row>
     <row r="4" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -2344,27 +2344,27 @@
         <v>1</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O4" s="27" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="P4" s="27" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Q4" s="26"/>
     </row>
     <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -2372,16 +2372,16 @@
         <v>1</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="O5" s="27" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="P5" s="27" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
@@ -2650,7 +2650,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2679,7 +2679,7 @@
         <v>80</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -2690,7 +2690,7 @@
         <v>116</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2698,7 +2698,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C4" s="6"/>
     </row>
@@ -2715,13 +2715,13 @@
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
-        <v>118</v>
+        <v>177</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>119</v>
+        <v>178</v>
       </c>
       <c r="C6" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="64" x14ac:dyDescent="0.2">
@@ -2729,7 +2729,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C7" s="6">
         <v>0</v>
@@ -2737,21 +2737,21 @@
     </row>
     <row r="8" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C9" s="6">
         <v>150</v>
@@ -2759,10 +2759,10 @@
     </row>
     <row r="10" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C10" s="6">
         <v>-75</v>
@@ -2770,10 +2770,10 @@
     </row>
     <row r="11" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C11" s="6">
         <v>0.01</v>
@@ -2795,10 +2795,10 @@
         <v>117</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2806,10 +2806,10 @@
         <v>55</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2817,10 +2817,10 @@
         <v>8</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2828,10 +2828,10 @@
         <v>7</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2839,21 +2839,21 @@
         <v>9</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2861,10 +2861,10 @@
         <v>28</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2872,10 +2872,10 @@
         <v>70</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2883,29 +2883,29 @@
         <v>76</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C23" s="11"/>
     </row>
@@ -2914,7 +2914,7 @@
         <v>75</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C24" s="6">
         <v>0</v>
@@ -2922,10 +2922,10 @@
     </row>
     <row r="25" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C25" s="6"/>
     </row>
@@ -2934,16 +2934,16 @@
         <v>114</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C26" s="6"/>
     </row>
     <row r="27" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C27" s="6"/>
     </row>
@@ -2998,7 +2998,7 @@
         <v>81</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Adding some output sub folder names to sub_dirs option
</commit_message>
<xml_diff>
--- a/config/config-sra-test-subset.xlsx
+++ b/config/config-sra-test-subset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cherikhsr/Documents/GitHub/cidc_atac/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59F5217-B2FD-EA4F-8508-EAE8B5A952A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC46466D-4EDB-8245-99CC-4831F4E48953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="500" windowWidth="30180" windowHeight="26500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1583,9 +1583,6 @@
     <t>/home/cherikhsr_nih_gov/atac_test_output/analysis</t>
   </si>
   <si>
-    <t>benchmark log info progress genome annot input cutadapt rqual_filter bam rseqc fastqc cnv peak chipqc</t>
-  </si>
-  <si>
     <t>gs://chips2-test-data/atac-test-sample-fastq/SRR16579104_1.fastq.gz</t>
   </si>
   <si>
@@ -1618,6 +1615,9 @@
   </si>
   <si>
     <t>narrow</t>
+  </si>
+  <si>
+    <t>benchmark log info progress genome annot input cutadapt rqual_filter bam rseqc fastqc cnv peak chipqc ptw track</t>
   </si>
 </sst>
 </file>
@@ -2350,10 +2350,10 @@
         <v>158</v>
       </c>
       <c r="O4" s="27" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="P4" s="27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Q4" s="26"/>
     </row>
@@ -2378,10 +2378,10 @@
         <v>160</v>
       </c>
       <c r="O5" s="27" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P5" s="27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
@@ -2650,14 +2650,14 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="77.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.83203125" customWidth="1"/>
+    <col min="3" max="3" width="84" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -2690,7 +2690,7 @@
         <v>116</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2715,10 +2715,10 @@
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="B6" s="25" t="s">
         <v>177</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>178</v>
       </c>
       <c r="C6" s="6">
         <v>1</v>
@@ -2743,7 +2743,7 @@
         <v>148</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="48" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add param for genome tracks region
</commit_message>
<xml_diff>
--- a/config/config-sra-test-subset.xlsx
+++ b/config/config-sra-test-subset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cherikhsr/Documents/GitHub/cidc_atac/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC46466D-4EDB-8245-99CC-4831F4E48953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67797DD9-3EA2-4048-819C-C30BA1A1ACB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="30180" windowHeight="26500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2920" yWindow="520" windowWidth="30180" windowHeight="26500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="183">
   <si>
     <t>&lt;string&gt;</t>
   </si>
@@ -1577,47 +1577,90 @@
     <t>Fastq File name (uncompressed or gzip compressed); For local files use path from root; for Amazon S3 files, use s3://&lt;bucket&gt;/&lt;key&gt;; for SRA runs, use the accession number (i.e. SRR2057712). Files separated by semi-colons will be merged before processing. If using SRR that are paired end copy the same accession into the fastq_file_2 column as well</t>
   </si>
   <si>
+    <t>gs://chips2-test-data/atac-test-sample-fastq/SRR16579104_1.fastq.gz</t>
+  </si>
+  <si>
+    <t>gs://chips2-test-data/atac-test-sample-fastq/SRR16579106_1.fastq.gz</t>
+  </si>
+  <si>
+    <t>gs://chips2-test-data/atac-test-sample-fastq/SRR16579104_2.fastq.gz</t>
+  </si>
+  <si>
+    <t>gs://chips2-test-data/atac-test-sample-fastq/SRR16579106_2.fastq.gz</t>
+  </si>
+  <si>
+    <t>run_genome_track</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Generate genomic track files and images. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Available options: 0;1   (REQUIRED)</t>
+    </r>
+  </si>
+  <si>
+    <t>narrow</t>
+  </si>
+  <si>
+    <t>benchmark log info progress genome annot input cutadapt rqual_filter bam rseqc fastqc cnv peak chipqc ptw track</t>
+  </si>
+  <si>
+    <t>track_region</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Genomic region to plot genome tracks over. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Example: chr1:500000-900000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(REQUIRED if run_genome_track)</t>
+    </r>
+  </si>
+  <si>
     <t>/home/cherikhsr_nih_gov/atac_test_output</t>
   </si>
   <si>
     <t>/home/cherikhsr_nih_gov/atac_test_output/analysis</t>
   </si>
   <si>
-    <t>gs://chips2-test-data/atac-test-sample-fastq/SRR16579104_1.fastq.gz</t>
-  </si>
-  <si>
-    <t>gs://chips2-test-data/atac-test-sample-fastq/SRR16579106_1.fastq.gz</t>
-  </si>
-  <si>
-    <t>gs://chips2-test-data/atac-test-sample-fastq/SRR16579104_2.fastq.gz</t>
-  </si>
-  <si>
-    <t>gs://chips2-test-data/atac-test-sample-fastq/SRR16579106_2.fastq.gz</t>
-  </si>
-  <si>
-    <t>run_genome_track</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Generate genomic track files and images. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Available options: 0;1   (REQUIRED)</t>
-    </r>
-  </si>
-  <si>
-    <t>narrow</t>
-  </si>
-  <si>
-    <t>benchmark log info progress genome annot input cutadapt rqual_filter bam rseqc fastqc cnv peak chipqc ptw track</t>
+    <t>chr1:750000-1050000</t>
   </si>
 </sst>
 </file>
@@ -2350,10 +2393,10 @@
         <v>158</v>
       </c>
       <c r="O4" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="P4" s="27" t="s">
         <v>172</v>
-      </c>
-      <c r="P4" s="27" t="s">
-        <v>174</v>
       </c>
       <c r="Q4" s="26"/>
     </row>
@@ -2378,10 +2421,10 @@
         <v>160</v>
       </c>
       <c r="O5" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="P5" s="27" t="s">
         <v>173</v>
-      </c>
-      <c r="P5" s="27" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
@@ -2647,10 +2690,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2679,7 +2722,7 @@
         <v>80</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -2690,7 +2733,7 @@
         <v>116</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2715,10 +2758,10 @@
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C6" s="6">
         <v>1</v>
@@ -2743,7 +2786,7 @@
         <v>148</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -2779,182 +2822,193 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>30</v>
+        <v>178</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" s="6">
-        <v>110</v>
+        <v>179</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="6">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B14" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C14" s="6" t="s">
         <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>124</v>
+        <v>137</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>118</v>
+        <v>9</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>28</v>
+        <v>118</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C21" s="6" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B23" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C23" s="11" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
+    <row r="24" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B24" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="C23" s="11"/>
-    </row>
-    <row r="24" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+      <c r="C24" s="11"/>
+    </row>
+    <row r="25" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C25" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C25" s="6"/>
     </row>
     <row r="26" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C26" s="6"/>
-    </row>
-    <row r="27" spans="1:3" ht="64" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C27" s="6"/>
-    </row>
-    <row r="28" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C29" s="6">
         <v>20</v>
       </c>
     </row>
@@ -2968,8 +3022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2998,7 +3052,7 @@
         <v>81</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">

</xml_diff>